<commit_message>
echoMRI editions in timedura column and CD1 exploration updates
</commit_message>
<xml_diff>
--- a/data/echoMRI/Kotz08012025.xlsx
+++ b/data/echoMRI/Kotz08012025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/data/echoMRI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcaballero/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DDE91CE-3DAA-F74B-B653-03937DBA4D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98353E42-5097-8146-961F-9459C3CC91AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractedScans" sheetId="1" r:id="rId1"/>
@@ -58,178 +58,178 @@
     <t>9367</t>
   </si>
   <si>
-    <t>10:57:20; 1 Aug 2025; 32; ems</t>
-  </si>
-  <si>
     <t>9361</t>
   </si>
   <si>
-    <t>10:59:29; 1 Aug 2025; 27; ems</t>
-  </si>
-  <si>
     <t>9377</t>
   </si>
   <si>
-    <t>11:01:06; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9372</t>
   </si>
   <si>
-    <t>11:02:33; 1 Aug 2025; 41; ems</t>
-  </si>
-  <si>
     <t>9373</t>
   </si>
   <si>
-    <t>11:03:54; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9374</t>
   </si>
   <si>
-    <t>11:05:31; 1 Aug 2025; 27; ems</t>
-  </si>
-  <si>
     <t>9378</t>
   </si>
   <si>
-    <t>11:06:46; 1 Aug 2025; 41; ems</t>
-  </si>
-  <si>
     <t>9375</t>
   </si>
   <si>
-    <t>11:08:04; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9369</t>
   </si>
   <si>
-    <t>11:09:19; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9355</t>
   </si>
   <si>
-    <t>11:10:30; 1 Aug 2025; 27; ems</t>
-  </si>
-  <si>
     <t>9357</t>
   </si>
   <si>
-    <t>11:11:33; 1 Aug 2025; 36; ems</t>
-  </si>
-  <si>
     <t>9358</t>
   </si>
   <si>
-    <t>11:13:01; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9370</t>
   </si>
   <si>
-    <t>11:14:23; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9360</t>
   </si>
   <si>
-    <t>11:15:30; 1 Aug 2025; 27; ems</t>
-  </si>
-  <si>
     <t>9362</t>
   </si>
   <si>
-    <t>11:16:29; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9359</t>
   </si>
   <si>
-    <t>11:17:57; 1 Aug 2025; 36; ems</t>
-  </si>
-  <si>
     <t>9356</t>
   </si>
   <si>
-    <t>11:19:05; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9376</t>
   </si>
   <si>
-    <t>11:20:16; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>7872</t>
   </si>
   <si>
-    <t>11:21:18; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>7873</t>
   </si>
   <si>
-    <t>11:22:47; 1 Aug 2025; 32; ems</t>
-  </si>
-  <si>
     <t>9353</t>
   </si>
   <si>
-    <t>11:24:08; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9366</t>
   </si>
   <si>
-    <t>11:25:13; 1 Aug 2025; 27; ems</t>
-  </si>
-  <si>
     <t>9364</t>
   </si>
   <si>
-    <t>11:26:16; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>9363</t>
   </si>
   <si>
-    <t>11:27:19; 1 Aug 2025; 32; ems</t>
-  </si>
-  <si>
     <t>7874</t>
   </si>
   <si>
-    <t>11:28:29; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>7876</t>
   </si>
   <si>
-    <t>11:29:49; 1 Aug 2025; 27; ems</t>
-  </si>
-  <si>
     <t>7867</t>
   </si>
   <si>
-    <t>11:31:01; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
     <t>7875</t>
   </si>
   <si>
-    <t>11:32:13; 1 Aug 2025; 27; ems</t>
-  </si>
-  <si>
     <t>9354</t>
   </si>
   <si>
-    <t>11:33:33; 1 Aug 2025; 31; ems</t>
-  </si>
-  <si>
-    <t>11:34:42; 1 Aug 2025; 31; ems</t>
+    <t>10:57:20 Aug 1, 2025; 32; ems</t>
+  </si>
+  <si>
+    <t>10:59:29 Aug 1, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>11:01:06 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:02:33 Aug 1, 2025; 41; ems</t>
+  </si>
+  <si>
+    <t>11:03:54 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:05:31 Aug 1, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>11:06:46 Aug 1, 2025; 41; ems</t>
+  </si>
+  <si>
+    <t>11:08:04 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:09:19 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:10:30 Aug 1, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>11:11:33 Aug 1, 2025; 36; ems</t>
+  </si>
+  <si>
+    <t>11:13:01 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:14:23 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:15:30 Aug 1, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>11:16:29 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:17:57 Aug 1, 2025; 36; ems</t>
+  </si>
+  <si>
+    <t>11:19:05 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:20:16 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:21:18 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:22:47 Aug 1, 2025; 32; ems</t>
+  </si>
+  <si>
+    <t>11:24:08 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:26:16 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:27:19 Aug 1, 2025; 32; ems</t>
+  </si>
+  <si>
+    <t>11:28:29 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:29:49 Aug 1, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>11:31:01 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:32:13 Aug 1, 2025; 27; ems</t>
+  </si>
+  <si>
+    <t>11:33:33 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:34:42 Aug 1, 2025; 31; ems</t>
+  </si>
+  <si>
+    <t>11:25:13 Aug 1, 2025; 27; ems</t>
   </si>
 </sst>
 </file>
@@ -570,9 +570,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
+  <cols>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -626,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -640,7 +645,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>18.77</v>
@@ -655,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -669,7 +674,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>5.56</v>
@@ -684,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -698,7 +703,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>3.18</v>
@@ -713,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -727,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>9.5299999999999994</v>
@@ -742,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -756,7 +761,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>13.8</v>
@@ -771,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -785,7 +790,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1.43</v>
@@ -800,7 +805,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -814,7 +819,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>0.96</v>
@@ -829,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -843,7 +848,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>7.8</v>
@@ -858,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -872,7 +877,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>8.2100000000000009</v>
@@ -887,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -901,7 +906,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>6.23</v>
@@ -916,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -930,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>22.12</v>
@@ -945,7 +950,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -959,7 +964,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>6.48</v>
@@ -974,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -988,7 +993,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>3.35</v>
@@ -1003,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1017,7 +1022,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>9.73</v>
@@ -1032,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1046,7 +1051,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>1.2</v>
@@ -1061,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1075,7 +1080,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>7.04</v>
@@ -1090,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1104,7 +1109,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>0.09</v>
@@ -1119,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1133,7 +1138,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>2.2599999999999998</v>
@@ -1148,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1162,7 +1167,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C21">
         <v>16.7</v>
@@ -1177,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1191,7 +1196,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>13.87</v>
@@ -1206,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1220,7 +1225,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>6.52</v>
@@ -1235,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1249,7 +1254,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>11.71</v>
@@ -1264,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1278,7 +1283,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>2.79</v>
@@ -1293,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1307,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>2.02</v>
@@ -1322,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1336,7 +1341,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>7.67</v>
@@ -1351,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1365,7 +1370,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>19.91</v>
@@ -1380,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1394,7 +1399,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C29">
         <v>7.24</v>
@@ -1423,7 +1428,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C30">
         <v>9.4499999999999993</v>
@@ -1438,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1467,7 +1472,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H31">
         <v>1</v>

</xml_diff>